<commit_message>
Stats - add xlsx with aggregated results from systemio
</commit_message>
<xml_diff>
--- a/docs/ReportAnalyzer-Final/2017-04-15-aggregated-BH-100-runs.xlsx
+++ b/docs/ReportAnalyzer-Final/2017-04-15-aggregated-BH-100-runs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -993,12 +993,12 @@
   <dimension ref="A1:CZ33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="94.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="91.42578125" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
@@ -1021,15 +1021,15 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <f>MIN(E2:CZ2)</f>
+        <f t="shared" ref="B2:B30" si="0">MIN(E2:CZ2)</f>
         <v>2.0070000000000001</v>
       </c>
       <c r="C2">
-        <f>MAX(E2:CZ2)</f>
+        <f t="shared" ref="C2:C30" si="1">MAX(E2:CZ2)</f>
         <v>4.2489999999999997</v>
       </c>
       <c r="D2" s="1">
-        <f>TRIMMEAN(E2:CZ2,B$33)</f>
+        <f t="shared" ref="D2:D30" si="2">TRIMMEAN(E2:CZ2,B$33)</f>
         <v>2.8380714285714292</v>
       </c>
       <c r="E2">
@@ -1338,15 +1338,15 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <f>MIN(E3:CZ3)</f>
+        <f t="shared" si="0"/>
         <v>0.82099999999999995</v>
       </c>
       <c r="C3">
-        <f>MAX(E3:CZ3)</f>
+        <f t="shared" si="1"/>
         <v>1.7390000000000001</v>
       </c>
       <c r="D3" s="1">
-        <f>TRIMMEAN(E3:CZ3,B$33)</f>
+        <f t="shared" si="2"/>
         <v>1.0875285714285714</v>
       </c>
       <c r="E3">
@@ -1655,15 +1655,15 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <f>MIN(E4:CZ4)</f>
+        <f t="shared" si="0"/>
         <v>0.59599999999999997</v>
       </c>
       <c r="C4" s="2">
-        <f>MAX(E4:CZ4)</f>
+        <f t="shared" si="1"/>
         <v>1.2490000000000001</v>
       </c>
       <c r="D4" s="3">
-        <f>TRIMMEAN(E4:CZ4,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.69540000000000013</v>
       </c>
       <c r="E4" s="2">
@@ -1972,15 +1972,15 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <f>MIN(E5:CZ5)</f>
+        <f t="shared" si="0"/>
         <v>0.46700000000000003</v>
       </c>
       <c r="C5">
-        <f>MAX(E5:CZ5)</f>
+        <f t="shared" si="1"/>
         <v>1.5660000000000001</v>
       </c>
       <c r="D5" s="1">
-        <f>TRIMMEAN(E5:CZ5,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.65165714285714282</v>
       </c>
       <c r="E5">
@@ -2289,15 +2289,15 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <f>MIN(E6:CZ6)</f>
+        <f t="shared" si="0"/>
         <v>0.158</v>
       </c>
       <c r="C6">
-        <f>MAX(E6:CZ6)</f>
+        <f t="shared" si="1"/>
         <v>0.84</v>
       </c>
       <c r="D6" s="1">
-        <f>TRIMMEAN(E6:CZ6,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.27800000000000002</v>
       </c>
       <c r="E6">
@@ -2606,15 +2606,15 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <f>MIN(E7:CZ7)</f>
+        <f t="shared" si="0"/>
         <v>0.17599999999999999</v>
       </c>
       <c r="C7">
-        <f>MAX(E7:CZ7)</f>
+        <f t="shared" si="1"/>
         <v>1.0980000000000001</v>
       </c>
       <c r="D7" s="1">
-        <f>TRIMMEAN(E7:CZ7,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.25682857142857146</v>
       </c>
       <c r="E7">
@@ -2923,15 +2923,15 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <f>MIN(E8:CZ8)</f>
+        <f t="shared" si="0"/>
         <v>0.20499999999999999</v>
       </c>
       <c r="C8">
-        <f>MAX(E8:CZ8)</f>
+        <f t="shared" si="1"/>
         <v>0.82299999999999995</v>
       </c>
       <c r="D8" s="1">
-        <f>TRIMMEAN(E8:CZ8,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.25404285714285707</v>
       </c>
       <c r="E8">
@@ -3240,15 +3240,15 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <f>MIN(E9:CZ9)</f>
+        <f t="shared" si="0"/>
         <v>0.155</v>
       </c>
       <c r="C9">
-        <f>MAX(E9:CZ9)</f>
+        <f t="shared" si="1"/>
         <v>0.86099999999999999</v>
       </c>
       <c r="D9" s="1">
-        <f>TRIMMEAN(E9:CZ9,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.22564285714285712</v>
       </c>
       <c r="E9">
@@ -3557,15 +3557,15 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <f>MIN(E10:CZ10)</f>
+        <f t="shared" si="0"/>
         <v>0.17399999999999999</v>
       </c>
       <c r="C10">
-        <f>MAX(E10:CZ10)</f>
+        <f t="shared" si="1"/>
         <v>0.78200000000000003</v>
       </c>
       <c r="D10" s="1">
-        <f>TRIMMEAN(E10:CZ10,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.20712857142857144</v>
       </c>
       <c r="E10">
@@ -3874,15 +3874,15 @@
         <v>17</v>
       </c>
       <c r="B11">
-        <f>MIN(E11:CZ11)</f>
+        <f t="shared" si="0"/>
         <v>0.161</v>
       </c>
       <c r="C11">
-        <f>MAX(E11:CZ11)</f>
+        <f t="shared" si="1"/>
         <v>0.68700000000000006</v>
       </c>
       <c r="D11" s="1">
-        <f>TRIMMEAN(E11:CZ11,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.19782857142857146</v>
       </c>
       <c r="E11">
@@ -4191,15 +4191,15 @@
         <v>23</v>
       </c>
       <c r="B12">
-        <f>MIN(E12:CZ12)</f>
+        <f t="shared" si="0"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="C12">
-        <f>MAX(E12:CZ12)</f>
+        <f t="shared" si="1"/>
         <v>0.70299999999999996</v>
       </c>
       <c r="D12" s="1">
-        <f>TRIMMEAN(E12:CZ12,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.19311428571428568</v>
       </c>
       <c r="E12">
@@ -4508,15 +4508,15 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <f>MIN(E13:CZ13)</f>
+        <f t="shared" si="0"/>
         <v>0.13900000000000001</v>
       </c>
       <c r="C13">
-        <f>MAX(E13:CZ13)</f>
+        <f t="shared" si="1"/>
         <v>0.70099999999999996</v>
       </c>
       <c r="D13" s="1">
-        <f>TRIMMEAN(E13:CZ13,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.19174285714285721</v>
       </c>
       <c r="E13">
@@ -4825,15 +4825,15 @@
         <v>8</v>
       </c>
       <c r="B14">
-        <f>MIN(E14:CZ14)</f>
+        <f t="shared" si="0"/>
         <v>0.13700000000000001</v>
       </c>
       <c r="C14">
-        <f>MAX(E14:CZ14)</f>
+        <f t="shared" si="1"/>
         <v>0.57499999999999996</v>
       </c>
       <c r="D14" s="1">
-        <f>TRIMMEAN(E14:CZ14,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.19047142857142854</v>
       </c>
       <c r="E14">
@@ -5142,15 +5142,15 @@
         <v>21</v>
       </c>
       <c r="B15">
-        <f>MIN(E15:CZ15)</f>
+        <f t="shared" si="0"/>
         <v>0.14299999999999999</v>
       </c>
       <c r="C15">
-        <f>MAX(E15:CZ15)</f>
+        <f t="shared" si="1"/>
         <v>0.78900000000000003</v>
       </c>
       <c r="D15" s="1">
-        <f>TRIMMEAN(E15:CZ15,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.18772857142857144</v>
       </c>
       <c r="E15">
@@ -5459,15 +5459,15 @@
         <v>7</v>
       </c>
       <c r="B16">
-        <f>MIN(E16:CZ16)</f>
+        <f t="shared" si="0"/>
         <v>0.14099999999999999</v>
       </c>
       <c r="C16">
-        <f>MAX(E16:CZ16)</f>
+        <f t="shared" si="1"/>
         <v>0.64300000000000002</v>
       </c>
       <c r="D16" s="1">
-        <f>TRIMMEAN(E16:CZ16,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.1802</v>
       </c>
       <c r="E16">
@@ -5776,15 +5776,15 @@
         <v>13</v>
       </c>
       <c r="B17">
-        <f>MIN(E17:CZ17)</f>
+        <f t="shared" si="0"/>
         <v>0.13900000000000001</v>
       </c>
       <c r="C17">
-        <f>MAX(E17:CZ17)</f>
+        <f t="shared" si="1"/>
         <v>0.57699999999999996</v>
       </c>
       <c r="D17" s="1">
-        <f>TRIMMEAN(E17:CZ17,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.17871428571428569</v>
       </c>
       <c r="E17">
@@ -6093,15 +6093,15 @@
         <v>2</v>
       </c>
       <c r="B18">
-        <f>MIN(E18:CZ18)</f>
+        <f t="shared" si="0"/>
         <v>0.13800000000000001</v>
       </c>
       <c r="C18">
-        <f>MAX(E18:CZ18)</f>
+        <f t="shared" si="1"/>
         <v>0.77</v>
       </c>
       <c r="D18" s="1">
-        <f>TRIMMEAN(E18:CZ18,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.17661428571428581</v>
       </c>
       <c r="E18">
@@ -6410,15 +6410,15 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <f>MIN(E19:CZ19)</f>
+        <f t="shared" si="0"/>
         <v>0.13700000000000001</v>
       </c>
       <c r="C19">
-        <f>MAX(E19:CZ19)</f>
+        <f t="shared" si="1"/>
         <v>0.67800000000000005</v>
       </c>
       <c r="D19" s="1">
-        <f>TRIMMEAN(E19:CZ19,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.16971428571428571</v>
       </c>
       <c r="E19">
@@ -6727,15 +6727,15 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <f>MIN(E20:CZ20)</f>
+        <f t="shared" si="0"/>
         <v>0.14199999999999999</v>
       </c>
       <c r="C20">
-        <f>MAX(E20:CZ20)</f>
+        <f t="shared" si="1"/>
         <v>0.64300000000000002</v>
       </c>
       <c r="D20" s="1">
-        <f>TRIMMEAN(E20:CZ20,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.16794285714285723</v>
       </c>
       <c r="E20">
@@ -7044,15 +7044,15 @@
         <v>5</v>
       </c>
       <c r="B21">
-        <f>MIN(E21:CZ21)</f>
+        <f t="shared" si="0"/>
         <v>0.13700000000000001</v>
       </c>
       <c r="C21">
-        <f>MAX(E21:CZ21)</f>
+        <f t="shared" si="1"/>
         <v>0.62</v>
       </c>
       <c r="D21" s="1">
-        <f>TRIMMEAN(E21:CZ21,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.16549999999999992</v>
       </c>
       <c r="E21">
@@ -7361,15 +7361,15 @@
         <v>10</v>
       </c>
       <c r="B22">
-        <f>MIN(E22:CZ22)</f>
+        <f t="shared" si="0"/>
         <v>0.13900000000000001</v>
       </c>
       <c r="C22">
-        <f>MAX(E22:CZ22)</f>
+        <f t="shared" si="1"/>
         <v>0.495</v>
       </c>
       <c r="D22" s="1">
-        <f>TRIMMEAN(E22:CZ22,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.16444285714285717</v>
       </c>
       <c r="E22">
@@ -7678,15 +7678,15 @@
         <v>20</v>
       </c>
       <c r="B23">
-        <f>MIN(E23:CZ23)</f>
+        <f t="shared" si="0"/>
         <v>0.13400000000000001</v>
       </c>
       <c r="C23">
-        <f>MAX(E23:CZ23)</f>
+        <f t="shared" si="1"/>
         <v>1.0449999999999999</v>
       </c>
       <c r="D23" s="1">
-        <f>TRIMMEAN(E23:CZ23,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.15909999999999994</v>
       </c>
       <c r="E23">
@@ -7995,15 +7995,15 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <f>MIN(E24:CZ24)</f>
+        <f t="shared" si="0"/>
         <v>0.13600000000000001</v>
       </c>
       <c r="C24">
-        <f>MAX(E24:CZ24)</f>
+        <f t="shared" si="1"/>
         <v>0.60599999999999998</v>
       </c>
       <c r="D24" s="1">
-        <f>TRIMMEAN(E24:CZ24,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.15765714285714297</v>
       </c>
       <c r="E24">
@@ -8312,15 +8312,15 @@
         <v>18</v>
       </c>
       <c r="B25">
-        <f>MIN(E25:CZ25)</f>
+        <f t="shared" si="0"/>
         <v>0.14199999999999999</v>
       </c>
       <c r="C25">
-        <f>MAX(E25:CZ25)</f>
+        <f t="shared" si="1"/>
         <v>0.77300000000000002</v>
       </c>
       <c r="D25" s="1">
-        <f>TRIMMEAN(E25:CZ25,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.15505714285714284</v>
       </c>
       <c r="E25">
@@ -8629,15 +8629,15 @@
         <v>15</v>
       </c>
       <c r="B26">
-        <f>MIN(E26:CZ26)</f>
+        <f t="shared" si="0"/>
         <v>0.13400000000000001</v>
       </c>
       <c r="C26">
-        <f>MAX(E26:CZ26)</f>
+        <f t="shared" si="1"/>
         <v>0.52400000000000002</v>
       </c>
       <c r="D26" s="1">
-        <f>TRIMMEAN(E26:CZ26,B$33)</f>
+        <f t="shared" si="2"/>
         <v>0.15192857142857133</v>
       </c>
       <c r="E26">
@@ -8946,15 +8946,15 @@
         <v>25</v>
       </c>
       <c r="B27" s="2">
-        <f>MIN(E27:CZ27)</f>
+        <f t="shared" si="0"/>
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="C27" s="2">
-        <f>MAX(E27:CZ27)</f>
+        <f t="shared" si="1"/>
         <v>0.54700000000000004</v>
       </c>
       <c r="D27" s="3">
-        <f>TRIMMEAN(E27:CZ27,B$33)</f>
+        <f t="shared" si="2"/>
         <v>7.6099999999999945E-2</v>
       </c>
       <c r="E27" s="2">
@@ -9263,15 +9263,15 @@
         <v>26</v>
       </c>
       <c r="B28" s="2">
-        <f>MIN(E28:CZ28)</f>
+        <f t="shared" si="0"/>
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="C28" s="2">
-        <f>MAX(E28:CZ28)</f>
+        <f t="shared" si="1"/>
         <v>0.27600000000000002</v>
       </c>
       <c r="D28" s="3">
-        <f>TRIMMEAN(E28:CZ28,B$33)</f>
+        <f t="shared" si="2"/>
         <v>4.1942857142857122E-2</v>
       </c>
       <c r="E28" s="2">
@@ -9580,15 +9580,15 @@
         <v>27</v>
       </c>
       <c r="B29" s="2">
-        <f>MIN(E29:CZ29)</f>
+        <f t="shared" si="0"/>
         <v>1.4E-2</v>
       </c>
       <c r="C29" s="2">
-        <f>MAX(E29:CZ29)</f>
+        <f t="shared" si="1"/>
         <v>0.27100000000000002</v>
       </c>
       <c r="D29" s="3">
-        <f>TRIMMEAN(E29:CZ29,B$33)</f>
+        <f t="shared" si="2"/>
         <v>1.5285714285714297E-2</v>
       </c>
       <c r="E29" s="2">
@@ -9897,15 +9897,15 @@
         <v>28</v>
       </c>
       <c r="B30" s="2">
-        <f>MIN(E30:CZ30)</f>
+        <f t="shared" si="0"/>
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C30" s="2">
-        <f>MAX(E30:CZ30)</f>
+        <f t="shared" si="1"/>
         <v>0.23</v>
       </c>
       <c r="D30" s="3">
-        <f>TRIMMEAN(E30:CZ30,B$33)</f>
+        <f t="shared" si="2"/>
         <v>6.8714285714285761E-3</v>
       </c>
       <c r="E30" s="2">

</xml_diff>